<commit_message>
ni 2004-2005 fix .45 fouten kruistabel 3C
</commit_message>
<xml_diff>
--- a/_data/ni/ni0405/individueel_eindstand_dworp_12_0405.xlsx
+++ b/_data/ni/ni0405/individueel_eindstand_dworp_12_0405.xlsx
@@ -1439,7 +1439,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O4:O15 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1585,7 +1585,7 @@
   <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O4:O15 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2411,7 +2411,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O4:O15 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3218,7 +3218,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O4:O15 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4016,7 +4016,7 @@
   <dimension ref="A1:AQ58"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="O4" activeCellId="0" sqref="O4:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4120,7 +4120,7 @@
       <c r="AC3" s="40"/>
       <c r="AD3" s="40"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="41" t="n">
         <v>1</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="41" t="n">
         <v>2</v>
       </c>
@@ -4422,7 +4422,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="41" t="n">
         <v>3</v>
       </c>
@@ -4562,7 +4562,7 @@
       </c>
       <c r="AO6" s="48" t="n">
         <f aca="false">L6+E13</f>
-        <v>5.95</v>
+        <v>6</v>
       </c>
       <c r="AP6" s="48" t="n">
         <f aca="false">M6+E14</f>
@@ -4570,10 +4570,10 @@
       </c>
       <c r="AQ6" s="56" t="n">
         <f aca="false">N6+E15</f>
-        <v>5.95</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="41" t="n">
         <v>4</v>
       </c>
@@ -4724,7 +4724,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="41" t="n">
         <v>5</v>
       </c>
@@ -4875,7 +4875,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="41" t="n">
         <v>6</v>
       </c>
@@ -5026,7 +5026,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="41" t="n">
         <v>7</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="41" t="n">
         <v>8</v>
       </c>
@@ -5328,7 +5328,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="41" t="n">
         <v>9</v>
       </c>
@@ -5479,7 +5479,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="n">
         <v>10</v>
       </c>
@@ -5493,7 +5493,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="44" t="n">
-        <v>2.45</v>
+        <v>2.5</v>
       </c>
       <c r="F13" s="44" t="n">
         <v>2.5</v>
@@ -5524,7 +5524,7 @@
       </c>
       <c r="O13" s="45" t="n">
         <f aca="false">SUM(C13:N13)</f>
-        <v>22.95</v>
+        <v>23</v>
       </c>
       <c r="P13" s="46" t="n">
         <f aca="false">SUM(S13:AD13)</f>
@@ -5592,7 +5592,7 @@
       </c>
       <c r="AH13" s="48" t="n">
         <f aca="false">E13+L6</f>
-        <v>5.95</v>
+        <v>6</v>
       </c>
       <c r="AI13" s="48" t="n">
         <f aca="false">F13+L7</f>
@@ -5630,7 +5630,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="41" t="n">
         <v>11</v>
       </c>
@@ -5781,7 +5781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="57" t="n">
         <v>12</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>0.5</v>
       </c>
       <c r="E15" s="59" t="n">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="F15" s="59" t="n">
         <v>1</v>
@@ -5826,7 +5826,7 @@
       </c>
       <c r="O15" s="61" t="n">
         <f aca="false">SUM(C15:N15)</f>
-        <v>12.45</v>
+        <v>12.5</v>
       </c>
       <c r="P15" s="62" t="n">
         <f aca="false">SUM(S15:AD15)</f>
@@ -5894,7 +5894,7 @@
       </c>
       <c r="AH15" s="40" t="n">
         <f aca="false">E15+N6</f>
-        <v>5.95</v>
+        <v>6</v>
       </c>
       <c r="AI15" s="40" t="n">
         <f aca="false">F15+N7</f>
@@ -11058,7 +11058,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O4:O15 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11856,7 +11856,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O4:O15 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12654,7 +12654,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="1" sqref="O4:O15 B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13452,7 +13452,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O4:O15 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14250,7 +14250,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O4:O15 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15048,7 +15048,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O4:O15 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15846,7 +15846,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O4:O15 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16644,7 +16644,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O4:O15 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>